<commit_message>
Data Driven Framework Listeners and ExtentReports
</commit_message>
<xml_diff>
--- a/target/test-classes/TutorialsNinja.xlsx
+++ b/target/test-classes/TutorialsNinja.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QAFox\BatchOne\DataDrivenFrameworkWorkspace\DDFProj\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A627673-ED84-42E3-89F9-C004C5F2F960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D344A5-339E-4388-B6B5-0E93F0EBD3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testcases" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
   <si>
     <t>TestCase</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>There is no product that matches the search criteria.</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -636,7 +639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -684,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CD3E39-C002-4FB9-9141-BDBB459D862D}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -837,7 +840,7 @@
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>10</v>

</xml_diff>